<commit_message>
add PPTs and school timetable
</commit_message>
<xml_diff>
--- a/schedule_and_school_timetable/school_timetable.xlsx
+++ b/schedule_and_school_timetable/school_timetable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_SHTU_\2324_summer\social_practise\Social_practise-group_of_teaching\schedule_and_school_timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AFE06C-BD34-4E31-857D-AE83D2061EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4D2921-D831-4BDA-BD53-76B6AAF438FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" tabRatio="594" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" tabRatio="594" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="七八年级课表" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">七八年级课表!$A$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -825,67 +826,115 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -894,61 +943,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1250,43 +1251,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="33"/>
-      <c r="B2" s="34">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11">
         <v>45503</v>
       </c>
-      <c r="C2" s="34">
+      <c r="C2" s="11">
         <v>45504</v>
       </c>
-      <c r="D2" s="34">
+      <c r="D2" s="11">
         <v>45505</v>
       </c>
-      <c r="E2" s="34">
+      <c r="E2" s="11">
         <v>45506</v>
       </c>
-      <c r="F2" s="34">
+      <c r="F2" s="11">
         <v>45507</v>
       </c>
-      <c r="G2" s="34">
+      <c r="G2" s="11">
         <v>45508</v>
       </c>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1298,14 +1299,14 @@
       <c r="E3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="16"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="9"/>
-      <c r="B4" s="8"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1315,29 +1316,29 @@
       <c r="E4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="17"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="18" t="s">
+      <c r="B5" s="30"/>
+      <c r="C5" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="21"/>
     </row>
     <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="2" t="s">
         <v>49</v>
       </c>
@@ -1355,60 +1356,60 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="27" t="s">
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="34" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A10" s="9"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="3" t="s">
         <v>34</v>
       </c>
@@ -1418,114 +1419,114 @@
       <c r="D10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="7"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="35"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="4" t="s">
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="28" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A12" s="9"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="24"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="36"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="42"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="16"/>
+      <c r="C14" s="7"/>
       <c r="D14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A15" s="5"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="17"/>
+      <c r="A15" s="38"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="6"/>
       <c r="D15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="21" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="22" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="21"/>
     </row>
     <row r="23" spans="1:7" ht="15.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="43"/>
-      <c r="B23" s="34">
+      <c r="A23" s="15"/>
+      <c r="B23" s="11">
         <v>45503</v>
       </c>
-      <c r="C23" s="34">
+      <c r="C23" s="11">
         <v>45504</v>
       </c>
-      <c r="D23" s="34">
+      <c r="D23" s="11">
         <v>45505</v>
       </c>
-      <c r="E23" s="34">
+      <c r="E23" s="11">
         <v>45506</v>
       </c>
-      <c r="F23" s="34">
+      <c r="F23" s="11">
         <v>45507</v>
       </c>
-      <c r="G23" s="34">
+      <c r="G23" s="11">
         <v>45508</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="12" t="s">
         <v>44</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -1542,9 +1543,9 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A25" s="9"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="36" t="s">
+      <c r="A25" s="29"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="3" t="s">
@@ -1561,23 +1562,23 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="44" t="s">
+      <c r="B26" s="30"/>
+      <c r="C26" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
     </row>
     <row r="27" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="8"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="2" t="s">
         <v>48</v>
       </c>
@@ -1590,11 +1591,11 @@
       <c r="F27" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G27" s="16"/>
+      <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A28" s="9"/>
-      <c r="B28" s="8"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="3" t="s">
         <v>15</v>
       </c>
@@ -1607,21 +1608,21 @@
       <c r="F28" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G28" s="17"/>
+      <c r="G28" s="6"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="21"/>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -1630,25 +1631,25 @@
       <c r="C30" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="39" t="s">
+      <c r="D30" s="14" t="s">
         <v>1</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F30" s="40" t="s">
+      <c r="F30" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="G30" s="28" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A31" s="9"/>
-      <c r="B31" s="27" t="s">
+      <c r="A31" s="29"/>
+      <c r="B31" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="27" t="s">
+      <c r="C31" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -1657,69 +1658,69 @@
       <c r="E31" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F31" s="41"/>
-      <c r="G31" s="9"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="29"/>
     </row>
     <row r="32" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="4" t="s">
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="28" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A33" s="9"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="9"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="29"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="20"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="21"/>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="16"/>
+      <c r="C35" s="7"/>
       <c r="D35" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E35" s="16"/>
+      <c r="E35" s="7"/>
       <c r="F35" s="2"/>
-      <c r="G35" s="16"/>
+      <c r="G35" s="7"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A36" s="5"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="17"/>
+      <c r="A36" s="38"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="6"/>
       <c r="D36" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E36" s="17"/>
+      <c r="E36" s="6"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="17"/>
+      <c r="G36" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A27" xr:uid="{E5070F60-1D8C-4FF2-B066-1BD1BF62E3A3}">
@@ -1728,20 +1729,6 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="30">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="B32:E33"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="B11:E12"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A9:A10"/>
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="A35:A36"/>
     <mergeCell ref="C26:G26"/>
@@ -1758,6 +1745,20 @@
     <mergeCell ref="F30:F33"/>
     <mergeCell ref="G30:G31"/>
     <mergeCell ref="G32:G33"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="B32:E33"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="B11:E12"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>